<commit_message>
Added column for secondary emotion
</commit_message>
<xml_diff>
--- a/data/Arie_testi.xlsx
+++ b/data/Arie_testi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0de618ced5d402fc/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fede9\source\repos\arieEmotions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{D5B7FAFB-70F7-4613-A165-F16346A1C7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2DE03C81-529C-4AFF-9405-91D336DA55E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45417F52-D718-45AD-9FE2-84E0934B07F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="562">
   <si>
     <t>Dovrei... Ma no..</t>
   </si>
@@ -1704,6 +1704,9 @@
   </si>
   <si>
     <t>ZAP1592516_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Emozione Sec.</t>
   </si>
 </sst>
 </file>
@@ -2556,22 +2559,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E372"/>
+  <dimension ref="A1:F372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="105.46484375" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" customWidth="1"/>
-    <col min="5" max="5" width="40.1328125" customWidth="1"/>
+    <col min="3" max="4" width="16.265625" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" customWidth="1"/>
+    <col min="6" max="6" width="40.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>265</v>
       </c>
@@ -2582,13 +2585,16 @@
         <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>289</v>
       </c>
@@ -2596,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>290</v>
       </c>
@@ -2604,7 +2610,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>291</v>
       </c>
@@ -2612,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>292</v>
       </c>
@@ -2620,7 +2626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>293</v>
       </c>
@@ -2628,7 +2634,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>295</v>
       </c>
@@ -2644,7 +2650,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>296</v>
       </c>
@@ -2652,7 +2658,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>297</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>298</v>
       </c>
@@ -2668,7 +2674,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>299</v>
       </c>
@@ -4777,19 +4783,19 @@
           <x14:formula1>
             <xm:f>emozioni!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C324:C1048576</xm:sqref>
+          <xm:sqref>C324:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F565519-F2A8-491A-B668-C89FCBDF9855}">
           <x14:formula1>
             <xm:f>emozioni!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D384</xm:sqref>
+          <xm:sqref>E2:E384</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9E620AF-DEF6-4D7F-8E96-A9ED41FA73EB}">
           <x14:formula1>
             <xm:f>emozioni!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C323</xm:sqref>
+          <xm:sqref>C2:D323</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>